<commit_message>
Update CMS Table Description
</commit_message>
<xml_diff>
--- a/HRMS/DashBoard Display Information (CMS)/Album.xlsx
+++ b/HRMS/DashBoard Display Information (CMS)/Album.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>Table Name -Album</t>
   </si>
   <si>
-    <t xml:space="preserve">Defination : </t>
-  </si>
-  <si>
     <t>S.No.</t>
   </si>
   <si>
@@ -104,13 +101,52 @@
   </si>
   <si>
     <t>LastUpdateByIp</t>
+  </si>
+  <si>
+    <t>For active or inactive record.</t>
+  </si>
+  <si>
+    <t>Get Login UserId .</t>
+  </si>
+  <si>
+    <t>Get Current Datetime when user Insert Record.</t>
+  </si>
+  <si>
+    <t>Keep IP Address of User System.</t>
+  </si>
+  <si>
+    <t>Get Current Datetime when user Update Record.</t>
+  </si>
+  <si>
+    <t>Get CurrentIP when user Update Record.</t>
+  </si>
+  <si>
+    <t>Get Login UserUd when User Update Record By IP Address.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defination :  इस फॉर्म के माद्यम </t>
+  </si>
+  <si>
+    <t>Primary id for auto increatment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get OfficeId  (MstOIS) in Numaric </t>
+  </si>
+  <si>
+    <t>Take Album Details as Input</t>
+  </si>
+  <si>
+    <t>Take input as date</t>
+  </si>
+  <si>
+    <t>Take Album Name as Input</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,13 +161,25 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -161,14 +209,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -178,6 +220,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +541,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,250 +550,274 @@
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="6" max="6" width="55" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="5" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>2</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>9</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>3</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>4</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>5</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="B13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>11</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>6</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>7</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>8</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>9</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="D15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>10</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>11</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>12</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="D16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="9" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>